<commit_message>
Update Data Access Layer
</commit_message>
<xml_diff>
--- a/ChiTietChucNang.xlsx
+++ b/ChiTietChucNang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NAM3\Quan-ly-dang-ky-hoc-phan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBD8A4C-248D-4C6D-927C-59EFBD1639DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3435FE4A-DED6-47E3-8462-5DF650747985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{346126DA-4C97-4AB5-8CDC-91EAC06DD919}"/>
+    <workbookView xWindow="-23112" yWindow="372" windowWidth="19008" windowHeight="12516" xr2:uid="{346126DA-4C97-4AB5-8CDC-91EAC06DD919}"/>
   </bookViews>
   <sheets>
     <sheet name="ChiTietChucNang" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="110">
   <si>
     <t>STT</t>
   </si>
@@ -332,13 +332,46 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>kiểu</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>nvarchar(100)</t>
+  </si>
+  <si>
+    <t>nvarchar(50)</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>smalldatetime</t>
+  </si>
+  <si>
+    <t>nvarchar(20)</t>
+  </si>
+  <si>
+    <t>nvarchar(1000)</t>
+  </si>
+  <si>
+    <t>nvarchar(10)</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>nvarchar(3000)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -354,6 +387,11 @@
     <font>
       <sz val="14"/>
       <color rgb="FF9C5700"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -408,7 +446,10 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -444,7 +485,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{924AB688-E7F2-40C1-B3BA-B9FA3E37ED6A}" name="Table1" displayName="Table1" ref="A1:C38" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{924AB688-E7F2-40C1-B3BA-B9FA3E37ED6A}" name="Table1" displayName="Table1" ref="A1:C38" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="A1:C38" xr:uid="{924AB688-E7F2-40C1-B3BA-B9FA3E37ED6A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{36E0526F-D463-41C5-803B-22E8DAD1B759}" name="Column1" dataDxfId="6"/>
@@ -456,13 +497,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2B54CA8-B4C4-4EE4-8BC5-AF0DB8C32C00}" name="Table2" displayName="Table2" ref="A1:B31" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:B31" xr:uid="{C2B54CA8-B4C4-4EE4-8BC5-AF0DB8C32C00}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2B54CA8-B4C4-4EE4-8BC5-AF0DB8C32C00}" name="Table2" displayName="Table2" ref="A1:C31" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C31" xr:uid="{C2B54CA8-B4C4-4EE4-8BC5-AF0DB8C32C00}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C107A559-4EEB-4CAE-8722-C72E9C528997}" name="Column1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{1D3323D1-32E5-4F35-BF73-3499ECB8AC7E}" name="Column2" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{E35155DD-C225-4F6C-9C10-8C7955ACE24C}" name="Column3" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -765,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3DE19F-B112-4244-806D-E761AE01BD83}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1130,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D0E92E-7305-47A7-8200-2D62ABF19F9F}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1143,207 +1185,297 @@
     <col min="3" max="3" width="47.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Xem học phần tích luỹ
</commit_message>
<xml_diff>
--- a/ChiTietChucNang.xlsx
+++ b/ChiTietChucNang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NAM3\Quan-ly-dang-ky-hoc-phan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249DB375-B93A-4676-8211-15EBED49D9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D677C6E2-BDC7-4959-9893-2A1417B823D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{346126DA-4C97-4AB5-8CDC-91EAC06DD919}"/>
+    <workbookView xWindow="-20796" yWindow="156" windowWidth="20532" windowHeight="12516" xr2:uid="{346126DA-4C97-4AB5-8CDC-91EAC06DD919}"/>
   </bookViews>
   <sheets>
     <sheet name="ChiTietChucNang" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="132">
   <si>
     <t>STT</t>
   </si>
@@ -199,33 +199,12 @@
     <t>Sinh viên có thể In kết quả phiếu đăng ký học phần</t>
   </si>
   <si>
-    <t>Thống kê</t>
-  </si>
-  <si>
-    <t>Tính học phí cho sinh viên</t>
-  </si>
-  <si>
-    <t>Quản trị hệ thống có thể tính học phí cho sinh viên dựa theo số tín chỉ mà sinh viên đã đăng ký</t>
-  </si>
-  <si>
     <t>Liệt kê danh sách sinh viên đăng ký môn học nào đó</t>
   </si>
   <si>
-    <t>Quản trị hệ thống có thể liệt kê danh sách sinh viên đăng ký môn học nào đó</t>
-  </si>
-  <si>
     <t>Lập danh sách thi cho môn học</t>
   </si>
   <si>
-    <t>Quản trị hệ thống có thể lập danh sách thi cho môn học</t>
-  </si>
-  <si>
-    <t>Thống kê số lượng sinh viên đăng ký từng môn</t>
-  </si>
-  <si>
-    <t>Quản trị hệ thống có thể thống kê số lượng sinh viên đăng ký theo từng môn</t>
-  </si>
-  <si>
     <t>Tên trường</t>
   </si>
   <si>
@@ -416,6 +395,42 @@
   </si>
   <si>
     <t>Ngày cập nhật</t>
+  </si>
+  <si>
+    <t>Xem lịch thi</t>
+  </si>
+  <si>
+    <t>Sinh viên có thể xem lịch thi của sinh viên trong học kỳ này</t>
+  </si>
+  <si>
+    <t>Xem học phí</t>
+  </si>
+  <si>
+    <t>Sinh viên xem học phí</t>
+  </si>
+  <si>
+    <t>Sinh viên có thể xem học phí của mình trong học kỳ này</t>
+  </si>
+  <si>
+    <t>Quản trị liệt kê danh sách sinh viên đăng ký môn học nào đó</t>
+  </si>
+  <si>
+    <t>Quản lý học vụ</t>
+  </si>
+  <si>
+    <t>Liệt kê học phần và số lượng sinh viên đã đăng ký của từng học phần</t>
+  </si>
+  <si>
+    <t>Quản trị hệ thống liệt kê học phần và số lượng đăng ký của từng học phần</t>
+  </si>
+  <si>
+    <t>Xuất danh sách sinh viên đăng ký học phần</t>
+  </si>
+  <si>
+    <t>Quản trị xuất danh sách sinh viên đăng ký học phần ra file excel</t>
+  </si>
+  <si>
+    <t>Quản trị lập danh sách thi cho môn học đã được sinh viên đăng ký</t>
   </si>
 </sst>
 </file>
@@ -447,7 +462,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +480,24 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -475,12 +508,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -491,9 +526,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -536,8 +585,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{924AB688-E7F2-40C1-B3BA-B9FA3E37ED6A}" name="Table1" displayName="Table1" ref="A1:C38" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:C38" xr:uid="{924AB688-E7F2-40C1-B3BA-B9FA3E37ED6A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{924AB688-E7F2-40C1-B3BA-B9FA3E37ED6A}" name="Table1" displayName="Table1" ref="A1:C45" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:C45" xr:uid="{924AB688-E7F2-40C1-B3BA-B9FA3E37ED6A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{36E0526F-D463-41C5-803B-22E8DAD1B759}" name="Column1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{74635C3B-5FC5-4204-8F4D-5D6385F30DAB}" name="Column2" dataDxfId="5"/>
@@ -856,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A3DE19F-B112-4244-806D-E761AE01BD83}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1071,19 +1120,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
+    <row r="23" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
         <v>1.5</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="3"/>
+      <c r="B23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>40</v>
@@ -1092,7 +1141,7 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>41</v>
@@ -1101,7 +1150,7 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>42</v>
@@ -1116,102 +1165,152 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
+    <row r="28" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7">
         <v>1.6</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="7"/>
+    </row>
+    <row r="29" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1" t="s">
+      <c r="C34" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
-        <v>2</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
         <v>2.1</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+    <row r="42" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="7"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1225,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D0E92E-7305-47A7-8200-2D62ABF19F9F}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1252,450 +1351,450 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Chức năng điều chỉnh học phần đã đăng ký
</commit_message>
<xml_diff>
--- a/ChiTietChucNang.xlsx
+++ b/ChiTietChucNang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NAM3\Quan-ly-dang-ky-hoc-phan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89037CB1-2D4A-4186-8132-D0E40C4B0D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A363CE-8BC2-4DE7-B752-2F55ADEEDD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2052" yWindow="156" windowWidth="20532" windowHeight="12516" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChiTietChucNang" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -451,8 +451,14 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,6 +494,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -498,14 +509,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -528,11 +540,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
     <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
+    <cellStyle name="Accent6" xfId="5" builtinId="49"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -897,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1084,29 +1101,29 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+      <c r="A20" s="10">
         <v>1.4</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1228,41 +1245,41 @@
       </c>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="3">
+    <row r="38" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="10">
         <v>2.1</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1" t="s">
+    <row r="39" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1" t="s">
+    <row r="40" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1" t="s">
+    <row r="41" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="10" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1314,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>

</xml_diff>